<commit_message>
modifica ai documenti per i test 3 e 4 aggiornamento del file data.json e report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS_SPA/DNLAB_THEMIS/3.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS_SPA/DNLAB_THEMIS/3.0.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\Documents\_Attività\_DNLAB_Statistiche\GIT_FSE20__\it-fse-accreditamento\GATEWAY\A1#111DEDALUS0000\DEDALUS_SPA\DNLAB_THEMIS\3.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97345928-FBF2-4EEE-B332-8581C1DD3851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA140B1-70CD-4851-8559-C4699337A842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="217" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="217" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -1824,24 +1824,6 @@
     <t>"2.16.840.1.113883.2.9.2.80110.4.4.1.7de0e15a7bcfae2dde807a3736442ea0767936052e052c14372c1c7df19accb2.5fbbc2fb49^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
   </si>
   <si>
-    <t>"2023-02-13T13:01:21Z"</t>
-  </si>
-  <si>
-    <t>"ec36c74e85e64fee"</t>
-  </si>
-  <si>
-    <t>"2.16.840.1.113883.2.9.2.80110.4.4.1.450b6b087834b58290fdddb6aba9bfe8f32a3b88eb31787ccdb4ca473e3ce1f4.15201cbe11^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
-  </si>
-  <si>
-    <t>"2023-02-13T13:01:41Z"</t>
-  </si>
-  <si>
-    <t>"9b569f7cbd554bc3"</t>
-  </si>
-  <si>
-    <t>"2.16.840.1.113883.2.9.2.80110.4.4.1.50f6654d35c4f0d3c542909db4ece051633482a684c4e3dae19eb1baa7f9fa64.992070eee0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
-  </si>
-  <si>
     <t>"2023-02-13T13:02:01Z"</t>
   </si>
   <si>
@@ -1963,6 +1945,24 @@
 La ratio della implementazione degli xmlcda qui inviati è che le stesse entità si trovino nelle medesime strutture nei vari casi possibili. 
 </t>
     </r>
+  </si>
+  <si>
+    <t>"2.16.840.1.113883.2.9.2.80110.4.4.1.7252b5d52d609477f181dcce18aa8f77069d241f3980198f96fa62cc22d6f8fb.ea5950669b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
+  </si>
+  <si>
+    <t>"3cbe83b5d9a9decb"</t>
+  </si>
+  <si>
+    <t>"2023-03-08T16:47:00Z"</t>
+  </si>
+  <si>
+    <t>"2023-03-08T16:46:00Z"</t>
+  </si>
+  <si>
+    <t>"b9090cfbb7776c1d"</t>
+  </si>
+  <si>
+    <t>"2.16.840.1.113883.2.9.2.80110.4.4.1.8f88398d958865dcab56b978fdee0d8eda5d4085a5692aa45deaa2a11ce14621.1971b22e8d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
   </si>
 </sst>
 </file>
@@ -2672,6 +2672,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2693,9 +2696,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2996,11 +2996,11 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="194.109375" customWidth="1"/>
-    <col min="3" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="194.140625" customWidth="1"/>
+    <col min="3" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -4067,30 +4067,30 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="58.5546875" customWidth="1"/>
-    <col min="5" max="5" width="33.109375" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" style="79" customWidth="1"/>
-    <col min="8" max="8" width="39.6640625" customWidth="1"/>
-    <col min="9" max="9" width="46.109375" style="77" customWidth="1"/>
-    <col min="10" max="10" width="50.5546875" customWidth="1"/>
-    <col min="11" max="11" width="27.33203125" customWidth="1"/>
-    <col min="12" max="12" width="33.33203125" customWidth="1"/>
-    <col min="13" max="13" width="45.5546875" customWidth="1"/>
-    <col min="14" max="14" width="41.44140625" style="54" customWidth="1"/>
-    <col min="15" max="15" width="31.6640625" customWidth="1"/>
-    <col min="16" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="79" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
+    <col min="9" max="9" width="46.140625" style="77" customWidth="1"/>
+    <col min="10" max="10" width="50.5703125" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" customWidth="1"/>
+    <col min="13" max="13" width="45.5703125" customWidth="1"/>
+    <col min="14" max="14" width="41.42578125" style="54" customWidth="1"/>
+    <col min="15" max="15" width="31.7109375" customWidth="1"/>
+    <col min="16" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -4105,15 +4105,15 @@
       <c r="N1" s="9"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="18">
-      <c r="A2" s="85" t="s">
+    <row r="2" spans="1:15" ht="18.75">
+      <c r="A2" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="87" t="s">
-        <v>369</v>
-      </c>
-      <c r="D2" s="86"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2" s="87"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -4125,15 +4125,15 @@
       <c r="N2" s="9"/>
       <c r="O2" s="6"/>
     </row>
-    <row r="3" spans="1:15" ht="15.6">
-      <c r="A3" s="88" t="s">
+    <row r="3" spans="1:15" ht="15.75">
+      <c r="A3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="94" t="s">
-        <v>370</v>
-      </c>
-      <c r="D3" s="86"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="95" t="s">
+        <v>364</v>
+      </c>
+      <c r="D3" s="87"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4145,13 +4145,13 @@
       <c r="N3" s="9"/>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:15" ht="15.6">
-      <c r="A4" s="90"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="94" t="s">
-        <v>371</v>
-      </c>
-      <c r="D4" s="86"/>
+    <row r="4" spans="1:15" ht="15.75">
+      <c r="A4" s="91"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="95" t="s">
+        <v>365</v>
+      </c>
+      <c r="D4" s="87"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -4164,13 +4164,13 @@
       <c r="N4" s="9"/>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="15.6">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="94" t="s">
-        <v>372</v>
-      </c>
-      <c r="D5" s="86"/>
+    <row r="5" spans="1:15" ht="15.75">
+      <c r="A5" s="93"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="95" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="87"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -4183,8 +4183,8 @@
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="83"/>
-      <c r="B6" s="84"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4212,7 +4212,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1">
+    <row r="8" spans="1:15" ht="15.75" thickBot="1">
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -4224,7 +4224,7 @@
       <c r="N8" s="50"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="36.6" thickBot="1">
+    <row r="9" spans="1:15" ht="38.25" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="47" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="10" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A10" s="38">
         <v>1</v>
       </c>
@@ -4308,11 +4308,11 @@
       </c>
       <c r="M10" s="45"/>
       <c r="N10" s="53"/>
-      <c r="O10" s="95" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="47" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+      <c r="O10" s="83" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A11" s="38">
         <v>2</v>
       </c>
@@ -4351,7 +4351,7 @@
       <c r="N11" s="53"/>
       <c r="O11" s="49"/>
     </row>
-    <row r="12" spans="1:15" s="47" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="12" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A12" s="38">
         <v>3</v>
       </c>
@@ -4368,16 +4368,16 @@
         <v>32</v>
       </c>
       <c r="F12" s="40">
-        <v>44970</v>
+        <v>44993</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>335</v>
+        <v>371</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>336</v>
+        <v>372</v>
       </c>
       <c r="I12" s="43" t="s">
-        <v>337</v>
+        <v>373</v>
       </c>
       <c r="J12" s="45"/>
       <c r="K12" s="45" t="s">
@@ -4390,7 +4390,7 @@
       <c r="N12" s="53"/>
       <c r="O12" s="49"/>
     </row>
-    <row r="13" spans="1:15" s="47" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="13" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A13" s="38">
         <v>4</v>
       </c>
@@ -4407,16 +4407,16 @@
         <v>34</v>
       </c>
       <c r="F13" s="40">
-        <v>44970</v>
+        <v>44993</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>338</v>
+        <v>370</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>339</v>
+        <v>369</v>
       </c>
       <c r="I13" s="43" t="s">
-        <v>340</v>
+        <v>368</v>
       </c>
       <c r="J13" s="45"/>
       <c r="K13" s="45" t="s">
@@ -4429,7 +4429,7 @@
       <c r="N13" s="53"/>
       <c r="O13" s="80"/>
     </row>
-    <row r="14" spans="1:15" s="47" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="14" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A14" s="38">
         <v>5</v>
       </c>
@@ -4449,13 +4449,13 @@
         <v>44970</v>
       </c>
       <c r="G14" s="42" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="H14" s="42" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="I14" s="43" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="J14" s="45"/>
       <c r="K14" s="45" t="s">
@@ -4468,7 +4468,7 @@
       <c r="N14" s="53"/>
       <c r="O14" s="82"/>
     </row>
-    <row r="15" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="15" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A15" s="13">
         <v>6</v>
       </c>
@@ -4495,7 +4495,7 @@
       <c r="N15" s="19"/>
       <c r="O15" s="81"/>
     </row>
-    <row r="16" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="16" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A16" s="13">
         <v>7</v>
       </c>
@@ -4522,7 +4522,7 @@
       <c r="N16" s="19"/>
       <c r="O16" s="20"/>
     </row>
-    <row r="17" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="17" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A17" s="13">
         <v>8</v>
       </c>
@@ -4549,7 +4549,7 @@
       <c r="N17" s="19"/>
       <c r="O17" s="20"/>
     </row>
-    <row r="18" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="18" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A18" s="13">
         <v>9</v>
       </c>
@@ -4576,7 +4576,7 @@
       <c r="N18" s="19"/>
       <c r="O18" s="20"/>
     </row>
-    <row r="19" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="19" spans="1:15" ht="405.75" hidden="1" thickBot="1">
       <c r="A19" s="13">
         <v>11</v>
       </c>
@@ -4603,7 +4603,7 @@
       <c r="N19" s="19"/>
       <c r="O19" s="20"/>
     </row>
-    <row r="20" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="20" spans="1:15" ht="405.75" hidden="1" thickBot="1">
       <c r="A20" s="13">
         <v>12</v>
       </c>
@@ -4630,7 +4630,7 @@
       <c r="N20" s="19"/>
       <c r="O20" s="20"/>
     </row>
-    <row r="21" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="21" spans="1:15" ht="405.75" hidden="1" thickBot="1">
       <c r="A21" s="13">
         <v>13</v>
       </c>
@@ -4657,7 +4657,7 @@
       <c r="N21" s="19"/>
       <c r="O21" s="20"/>
     </row>
-    <row r="22" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="22" spans="1:15" ht="405.75" hidden="1" thickBot="1">
       <c r="A22" s="13">
         <v>14</v>
       </c>
@@ -4684,7 +4684,7 @@
       <c r="N22" s="19"/>
       <c r="O22" s="20"/>
     </row>
-    <row r="23" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="23" spans="1:15" ht="405.75" hidden="1" thickBot="1">
       <c r="A23" s="13">
         <v>16</v>
       </c>
@@ -4711,7 +4711,7 @@
       <c r="N23" s="19"/>
       <c r="O23" s="20"/>
     </row>
-    <row r="24" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="24" spans="1:15" ht="405.75" hidden="1" thickBot="1">
       <c r="A24" s="13">
         <v>17</v>
       </c>
@@ -4738,7 +4738,7 @@
       <c r="N24" s="19"/>
       <c r="O24" s="20"/>
     </row>
-    <row r="25" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="25" spans="1:15" ht="405.75" hidden="1" thickBot="1">
       <c r="A25" s="13">
         <v>18</v>
       </c>
@@ -4765,7 +4765,7 @@
       <c r="N25" s="19"/>
       <c r="O25" s="20"/>
     </row>
-    <row r="26" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="26" spans="1:15" ht="405.75" hidden="1" thickBot="1">
       <c r="A26" s="13">
         <v>19</v>
       </c>
@@ -4792,7 +4792,7 @@
       <c r="N26" s="19"/>
       <c r="O26" s="20"/>
     </row>
-    <row r="27" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="27" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A27" s="13">
         <v>20</v>
       </c>
@@ -4819,7 +4819,7 @@
       <c r="N27" s="19"/>
       <c r="O27" s="20"/>
     </row>
-    <row r="28" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="28" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A28" s="13">
         <v>21</v>
       </c>
@@ -4846,7 +4846,7 @@
       <c r="N28" s="19"/>
       <c r="O28" s="20"/>
     </row>
-    <row r="29" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="29" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A29" s="13">
         <v>22</v>
       </c>
@@ -4873,7 +4873,7 @@
       <c r="N29" s="19"/>
       <c r="O29" s="20"/>
     </row>
-    <row r="30" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="30" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A30" s="13">
         <v>23</v>
       </c>
@@ -4900,7 +4900,7 @@
       <c r="N30" s="19"/>
       <c r="O30" s="20"/>
     </row>
-    <row r="31" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="31" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A31" s="13">
         <v>24</v>
       </c>
@@ -4927,7 +4927,7 @@
       <c r="N31" s="19"/>
       <c r="O31" s="20"/>
     </row>
-    <row r="32" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="32" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A32" s="13">
         <v>25</v>
       </c>
@@ -4954,7 +4954,7 @@
       <c r="N32" s="19"/>
       <c r="O32" s="20"/>
     </row>
-    <row r="33" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="33" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A33" s="13">
         <v>26</v>
       </c>
@@ -4981,7 +4981,7 @@
       <c r="N33" s="19"/>
       <c r="O33" s="20"/>
     </row>
-    <row r="34" spans="1:15" ht="389.4" hidden="1" thickBot="1">
+    <row r="34" spans="1:15" ht="409.6" hidden="1" thickBot="1">
       <c r="A34" s="13">
         <v>27</v>
       </c>
@@ -5008,7 +5008,7 @@
       <c r="N34" s="19"/>
       <c r="O34" s="20"/>
     </row>
-    <row r="35" spans="1:15" s="47" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="35" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A35" s="38">
         <v>28</v>
       </c>
@@ -5028,10 +5028,10 @@
         <v>44970</v>
       </c>
       <c r="G35" s="41" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="H35" s="42" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="I35" s="43" t="s">
         <v>322</v>
@@ -5051,7 +5051,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="36" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A36" s="13">
         <v>29</v>
       </c>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="O36" s="20"/>
     </row>
-    <row r="37" spans="1:15" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="37" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A37" s="13">
         <v>31</v>
       </c>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="O37" s="20"/>
     </row>
-    <row r="38" spans="1:15" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="38" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A38" s="13">
         <v>33</v>
       </c>
@@ -5138,7 +5138,7 @@
       </c>
       <c r="O38" s="20"/>
     </row>
-    <row r="39" spans="1:15" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="39" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A39" s="13">
         <v>34</v>
       </c>
@@ -5167,7 +5167,7 @@
       </c>
       <c r="O39" s="20"/>
     </row>
-    <row r="40" spans="1:15" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="40" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A40" s="13">
         <v>35</v>
       </c>
@@ -5196,7 +5196,7 @@
       </c>
       <c r="O40" s="20"/>
     </row>
-    <row r="41" spans="1:15" s="47" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="41" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A41" s="38">
         <v>36</v>
       </c>
@@ -5216,10 +5216,10 @@
         <v>44970</v>
       </c>
       <c r="G41" s="41" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="I41" s="43" t="s">
         <v>322</v>
@@ -5239,7 +5239,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="274.2" hidden="1" thickBot="1">
+    <row r="42" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A42" s="13">
         <v>37</v>
       </c>
@@ -5268,7 +5268,7 @@
       </c>
       <c r="O42" s="20"/>
     </row>
-    <row r="43" spans="1:15" ht="274.2" hidden="1" thickBot="1">
+    <row r="43" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A43" s="13">
         <v>39</v>
       </c>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="O43" s="20"/>
     </row>
-    <row r="44" spans="1:15" ht="274.2" hidden="1" thickBot="1">
+    <row r="44" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A44" s="13">
         <v>41</v>
       </c>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="O44" s="20"/>
     </row>
-    <row r="45" spans="1:15" ht="274.2" hidden="1" thickBot="1">
+    <row r="45" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A45" s="13">
         <v>42</v>
       </c>
@@ -5355,7 +5355,7 @@
       </c>
       <c r="O45" s="20"/>
     </row>
-    <row r="46" spans="1:15" ht="274.2" hidden="1" thickBot="1">
+    <row r="46" spans="1:15" ht="315.75" hidden="1" thickBot="1">
       <c r="A46" s="13">
         <v>43</v>
       </c>
@@ -5384,7 +5384,7 @@
       </c>
       <c r="O46" s="20"/>
     </row>
-    <row r="47" spans="1:15" s="47" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="47" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A47" s="38">
         <v>44</v>
       </c>
@@ -5419,7 +5419,7 @@
       </c>
       <c r="O47" s="49"/>
     </row>
-    <row r="48" spans="1:15" ht="87" hidden="1" thickBot="1">
+    <row r="48" spans="1:15" ht="105.75" hidden="1" thickBot="1">
       <c r="A48" s="13">
         <v>45</v>
       </c>
@@ -5448,7 +5448,7 @@
       </c>
       <c r="O48" s="20"/>
     </row>
-    <row r="49" spans="1:15" ht="87" hidden="1" thickBot="1">
+    <row r="49" spans="1:15" ht="105.75" hidden="1" thickBot="1">
       <c r="A49" s="13">
         <v>47</v>
       </c>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="O49" s="20"/>
     </row>
-    <row r="50" spans="1:15" ht="87" hidden="1" thickBot="1">
+    <row r="50" spans="1:15" ht="105.75" hidden="1" thickBot="1">
       <c r="A50" s="13">
         <v>49</v>
       </c>
@@ -5506,7 +5506,7 @@
       </c>
       <c r="O50" s="20"/>
     </row>
-    <row r="51" spans="1:15" ht="87" hidden="1" thickBot="1">
+    <row r="51" spans="1:15" ht="105.75" hidden="1" thickBot="1">
       <c r="A51" s="13">
         <v>50</v>
       </c>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="O51" s="20"/>
     </row>
-    <row r="52" spans="1:15" ht="87" hidden="1" thickBot="1">
+    <row r="52" spans="1:15" ht="105.75" hidden="1" thickBot="1">
       <c r="A52" s="13">
         <v>51</v>
       </c>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="O52" s="20"/>
     </row>
-    <row r="53" spans="1:15" s="65" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="53" spans="1:15" s="65" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A53" s="55">
         <v>52</v>
       </c>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="O53" s="64"/>
     </row>
-    <row r="54" spans="1:15" s="75" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="54" spans="1:15" s="75" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A54" s="66">
         <v>53</v>
       </c>
@@ -5619,13 +5619,13 @@
         <v>44970</v>
       </c>
       <c r="G54" s="78" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="H54" s="69" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="I54" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="J54" s="71" t="s">
         <v>325</v>
@@ -5638,7 +5638,7 @@
       <c r="N54" s="73"/>
       <c r="O54" s="74"/>
     </row>
-    <row r="55" spans="1:15" ht="241.8" customHeight="1" thickBot="1">
+    <row r="55" spans="1:15" ht="241.9" customHeight="1" thickBot="1">
       <c r="A55" s="13">
         <v>54</v>
       </c>
@@ -5658,13 +5658,13 @@
         <v>44970</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="I55" s="37" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="J55" s="44" t="s">
         <v>325</v>
@@ -5679,7 +5679,7 @@
       </c>
       <c r="O55" s="20"/>
     </row>
-    <row r="56" spans="1:15" ht="241.8" customHeight="1" thickBot="1">
+    <row r="56" spans="1:15" ht="241.9" customHeight="1" thickBot="1">
       <c r="A56" s="13">
         <v>55</v>
       </c>
@@ -5699,13 +5699,13 @@
         <v>44970</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="I56" s="37" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="J56" s="44" t="s">
         <v>325</v>
@@ -5720,7 +5720,7 @@
       </c>
       <c r="O56" s="20"/>
     </row>
-    <row r="57" spans="1:15" s="65" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="57" spans="1:15" s="65" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A57" s="55">
         <v>56</v>
       </c>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="O57" s="64"/>
     </row>
-    <row r="58" spans="1:15" ht="241.8" customHeight="1" thickBot="1">
+    <row r="58" spans="1:15" ht="241.9" customHeight="1" thickBot="1">
       <c r="A58" s="13">
         <v>57</v>
       </c>
@@ -5775,13 +5775,13 @@
         <v>44970</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="I58" s="37" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="J58" s="44" t="s">
         <v>325</v>
@@ -5796,7 +5796,7 @@
       </c>
       <c r="O58" s="20"/>
     </row>
-    <row r="59" spans="1:15" ht="241.8" customHeight="1" thickBot="1">
+    <row r="59" spans="1:15" ht="241.9" customHeight="1" thickBot="1">
       <c r="A59" s="13">
         <v>58</v>
       </c>
@@ -5816,13 +5816,13 @@
         <v>44970</v>
       </c>
       <c r="G59" s="17" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="I59" s="37" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="J59" s="44" t="s">
         <v>325</v>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="O59" s="20"/>
     </row>
-    <row r="60" spans="1:15" s="65" customFormat="1" ht="241.8" customHeight="1" thickBot="1">
+    <row r="60" spans="1:15" s="65" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
       <c r="A60" s="55">
         <v>59</v>
       </c>
@@ -5872,7 +5872,7 @@
       </c>
       <c r="O60" s="64"/>
     </row>
-    <row r="61" spans="1:15" ht="241.8" customHeight="1" thickBot="1">
+    <row r="61" spans="1:15" ht="241.9" customHeight="1" thickBot="1">
       <c r="A61" s="13">
         <v>60</v>
       </c>
@@ -5892,13 +5892,13 @@
         <v>44970</v>
       </c>
       <c r="G61" s="17" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="H61" s="17" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="I61" s="37" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="J61" s="44" t="s">
         <v>325</v>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="O61" s="20"/>
     </row>
-    <row r="62" spans="1:15" ht="241.8" customHeight="1" thickBot="1">
+    <row r="62" spans="1:15" ht="241.9" customHeight="1" thickBot="1">
       <c r="A62" s="13">
         <v>61</v>
       </c>
@@ -5933,13 +5933,13 @@
         <v>44970</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="I62" s="37" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="J62" s="44" t="s">
         <v>325</v>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="O62" s="20"/>
     </row>
-    <row r="63" spans="1:15" s="65" customFormat="1" ht="241.8" customHeight="1">
+    <row r="63" spans="1:15" s="65" customFormat="1" ht="241.9" customHeight="1">
       <c r="A63" s="55">
         <v>62</v>
       </c>
@@ -5989,7 +5989,7 @@
       </c>
       <c r="O63" s="64"/>
     </row>
-    <row r="64" spans="1:15" ht="316.8" hidden="1">
+    <row r="64" spans="1:15" ht="345" hidden="1">
       <c r="A64" s="13">
         <v>63</v>
       </c>
@@ -6018,7 +6018,7 @@
       </c>
       <c r="O64" s="20"/>
     </row>
-    <row r="65" spans="1:15" ht="316.8" hidden="1">
+    <row r="65" spans="1:15" ht="345" hidden="1">
       <c r="A65" s="13">
         <v>64</v>
       </c>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="O65" s="20"/>
     </row>
-    <row r="66" spans="1:15" ht="316.8" hidden="1">
+    <row r="66" spans="1:15" ht="345" hidden="1">
       <c r="A66" s="13">
         <v>65</v>
       </c>
@@ -6076,7 +6076,7 @@
       </c>
       <c r="O66" s="20"/>
     </row>
-    <row r="67" spans="1:15" ht="316.8" hidden="1">
+    <row r="67" spans="1:15" ht="345" hidden="1">
       <c r="A67" s="13">
         <v>66</v>
       </c>
@@ -6105,7 +6105,7 @@
       </c>
       <c r="O67" s="20"/>
     </row>
-    <row r="68" spans="1:15" ht="316.8" hidden="1">
+    <row r="68" spans="1:15" ht="345" hidden="1">
       <c r="A68" s="13">
         <v>67</v>
       </c>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="O68" s="20"/>
     </row>
-    <row r="69" spans="1:15" ht="316.8" hidden="1">
+    <row r="69" spans="1:15" ht="345" hidden="1">
       <c r="A69" s="13">
         <v>68</v>
       </c>
@@ -6163,7 +6163,7 @@
       </c>
       <c r="O69" s="20"/>
     </row>
-    <row r="70" spans="1:15" ht="316.8" hidden="1">
+    <row r="70" spans="1:15" ht="345" hidden="1">
       <c r="A70" s="13">
         <v>69</v>
       </c>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="O70" s="20"/>
     </row>
-    <row r="71" spans="1:15" ht="316.8" hidden="1">
+    <row r="71" spans="1:15" ht="345" hidden="1">
       <c r="A71" s="13">
         <v>70</v>
       </c>
@@ -6221,7 +6221,7 @@
       </c>
       <c r="O71" s="20"/>
     </row>
-    <row r="72" spans="1:15" ht="316.8" hidden="1">
+    <row r="72" spans="1:15" ht="345" hidden="1">
       <c r="A72" s="13">
         <v>71</v>
       </c>
@@ -6250,7 +6250,7 @@
       </c>
       <c r="O72" s="20"/>
     </row>
-    <row r="73" spans="1:15" ht="316.8" hidden="1">
+    <row r="73" spans="1:15" ht="345" hidden="1">
       <c r="A73" s="13">
         <v>72</v>
       </c>
@@ -6279,7 +6279,7 @@
       </c>
       <c r="O73" s="20"/>
     </row>
-    <row r="74" spans="1:15" ht="316.8" hidden="1">
+    <row r="74" spans="1:15" ht="345" hidden="1">
       <c r="A74" s="13">
         <v>73</v>
       </c>
@@ -6308,7 +6308,7 @@
       </c>
       <c r="O74" s="20"/>
     </row>
-    <row r="75" spans="1:15" ht="316.8" hidden="1">
+    <row r="75" spans="1:15" ht="345" hidden="1">
       <c r="A75" s="13">
         <v>74</v>
       </c>
@@ -6337,7 +6337,7 @@
       </c>
       <c r="O75" s="20"/>
     </row>
-    <row r="76" spans="1:15" ht="345.6" hidden="1">
+    <row r="76" spans="1:15" ht="360" hidden="1">
       <c r="A76" s="13">
         <v>75</v>
       </c>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="O76" s="20"/>
     </row>
-    <row r="77" spans="1:15" ht="331.2" hidden="1">
+    <row r="77" spans="1:15" ht="345" hidden="1">
       <c r="A77" s="13">
         <v>76</v>
       </c>
@@ -6395,7 +6395,7 @@
       </c>
       <c r="O77" s="20"/>
     </row>
-    <row r="78" spans="1:15" ht="316.8" hidden="1">
+    <row r="78" spans="1:15" ht="330" hidden="1">
       <c r="A78" s="13">
         <v>77</v>
       </c>
@@ -6424,7 +6424,7 @@
       </c>
       <c r="O78" s="20"/>
     </row>
-    <row r="79" spans="1:15" ht="316.8" hidden="1">
+    <row r="79" spans="1:15" ht="330" hidden="1">
       <c r="A79" s="13">
         <v>78</v>
       </c>
@@ -6453,7 +6453,7 @@
       </c>
       <c r="O79" s="20"/>
     </row>
-    <row r="80" spans="1:15" ht="331.2" hidden="1">
+    <row r="80" spans="1:15" ht="345" hidden="1">
       <c r="A80" s="13">
         <v>79</v>
       </c>
@@ -6482,7 +6482,7 @@
       </c>
       <c r="O80" s="20"/>
     </row>
-    <row r="81" spans="1:15" ht="331.2" hidden="1">
+    <row r="81" spans="1:15" ht="345" hidden="1">
       <c r="A81" s="13">
         <v>80</v>
       </c>
@@ -6511,7 +6511,7 @@
       </c>
       <c r="O81" s="20"/>
     </row>
-    <row r="82" spans="1:15" ht="331.2" hidden="1">
+    <row r="82" spans="1:15" ht="345" hidden="1">
       <c r="A82" s="13">
         <v>81</v>
       </c>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="O82" s="20"/>
     </row>
-    <row r="83" spans="1:15" ht="331.2" hidden="1">
+    <row r="83" spans="1:15" ht="345" hidden="1">
       <c r="A83" s="13">
         <v>82</v>
       </c>
@@ -6569,7 +6569,7 @@
       </c>
       <c r="O83" s="20"/>
     </row>
-    <row r="84" spans="1:15" ht="316.8" hidden="1">
+    <row r="84" spans="1:15" ht="330" hidden="1">
       <c r="A84" s="13">
         <v>83</v>
       </c>
@@ -6598,7 +6598,7 @@
       </c>
       <c r="O84" s="20"/>
     </row>
-    <row r="85" spans="1:15" ht="316.8" hidden="1">
+    <row r="85" spans="1:15" ht="330" hidden="1">
       <c r="A85" s="13">
         <v>84</v>
       </c>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="O85" s="20"/>
     </row>
-    <row r="86" spans="1:15" ht="331.2" hidden="1">
+    <row r="86" spans="1:15" ht="345" hidden="1">
       <c r="A86" s="13">
         <v>85</v>
       </c>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="O86" s="20"/>
     </row>
-    <row r="87" spans="1:15" ht="331.2" hidden="1">
+    <row r="87" spans="1:15" ht="345" hidden="1">
       <c r="A87" s="13">
         <v>86</v>
       </c>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="O87" s="20"/>
     </row>
-    <row r="88" spans="1:15" ht="345.6" hidden="1">
+    <row r="88" spans="1:15" ht="360" hidden="1">
       <c r="A88" s="13">
         <v>87</v>
       </c>
@@ -6714,7 +6714,7 @@
       </c>
       <c r="O88" s="20"/>
     </row>
-    <row r="89" spans="1:15" ht="331.2" hidden="1">
+    <row r="89" spans="1:15" ht="345" hidden="1">
       <c r="A89" s="13">
         <v>88</v>
       </c>
@@ -6743,7 +6743,7 @@
       </c>
       <c r="O89" s="20"/>
     </row>
-    <row r="90" spans="1:15" ht="316.8" hidden="1">
+    <row r="90" spans="1:15" ht="330" hidden="1">
       <c r="A90" s="13">
         <v>89</v>
       </c>
@@ -6772,7 +6772,7 @@
       </c>
       <c r="O90" s="20"/>
     </row>
-    <row r="91" spans="1:15" ht="316.8" hidden="1">
+    <row r="91" spans="1:15" ht="330" hidden="1">
       <c r="A91" s="13">
         <v>90</v>
       </c>
@@ -6801,7 +6801,7 @@
       </c>
       <c r="O91" s="20"/>
     </row>
-    <row r="92" spans="1:15" ht="331.2" hidden="1">
+    <row r="92" spans="1:15" ht="345" hidden="1">
       <c r="A92" s="13">
         <v>91</v>
       </c>
@@ -6830,7 +6830,7 @@
       </c>
       <c r="O92" s="20"/>
     </row>
-    <row r="93" spans="1:15" ht="331.2" hidden="1">
+    <row r="93" spans="1:15" ht="345" hidden="1">
       <c r="A93" s="13">
         <v>92</v>
       </c>
@@ -6859,7 +6859,7 @@
       </c>
       <c r="O93" s="20"/>
     </row>
-    <row r="94" spans="1:15" ht="331.2" hidden="1">
+    <row r="94" spans="1:15" ht="345" hidden="1">
       <c r="A94" s="13">
         <v>93</v>
       </c>
@@ -6888,7 +6888,7 @@
       </c>
       <c r="O94" s="20"/>
     </row>
-    <row r="95" spans="1:15" ht="331.2" hidden="1">
+    <row r="95" spans="1:15" ht="360" hidden="1">
       <c r="A95" s="13">
         <v>94</v>
       </c>
@@ -6917,7 +6917,7 @@
       </c>
       <c r="O95" s="20"/>
     </row>
-    <row r="96" spans="1:15" ht="331.2" hidden="1">
+    <row r="96" spans="1:15" ht="360" hidden="1">
       <c r="A96" s="13">
         <v>95</v>
       </c>
@@ -6946,7 +6946,7 @@
       </c>
       <c r="O96" s="20"/>
     </row>
-    <row r="97" spans="1:15" ht="302.39999999999998" hidden="1">
+    <row r="97" spans="1:15" ht="330" hidden="1">
       <c r="A97" s="13">
         <v>96</v>
       </c>
@@ -6975,7 +6975,7 @@
       </c>
       <c r="O97" s="20"/>
     </row>
-    <row r="98" spans="1:15" ht="316.8" hidden="1">
+    <row r="98" spans="1:15" ht="345" hidden="1">
       <c r="A98" s="13">
         <v>97</v>
       </c>
@@ -7004,7 +7004,7 @@
       </c>
       <c r="O98" s="20"/>
     </row>
-    <row r="99" spans="1:15" ht="331.2" hidden="1">
+    <row r="99" spans="1:15" ht="360" hidden="1">
       <c r="A99" s="13">
         <v>98</v>
       </c>
@@ -7033,7 +7033,7 @@
       </c>
       <c r="O99" s="20"/>
     </row>
-    <row r="100" spans="1:15" ht="331.2" hidden="1">
+    <row r="100" spans="1:15" ht="360" hidden="1">
       <c r="A100" s="13">
         <v>99</v>
       </c>
@@ -7062,7 +7062,7 @@
       </c>
       <c r="O100" s="20"/>
     </row>
-    <row r="101" spans="1:15" ht="302.39999999999998" hidden="1">
+    <row r="101" spans="1:15" ht="330" hidden="1">
       <c r="A101" s="13">
         <v>100</v>
       </c>
@@ -7091,7 +7091,7 @@
       </c>
       <c r="O101" s="20"/>
     </row>
-    <row r="102" spans="1:15" ht="316.8" hidden="1">
+    <row r="102" spans="1:15" ht="345" hidden="1">
       <c r="A102" s="13">
         <v>101</v>
       </c>
@@ -7120,7 +7120,7 @@
       </c>
       <c r="O102" s="20"/>
     </row>
-    <row r="103" spans="1:15" ht="331.2" hidden="1">
+    <row r="103" spans="1:15" ht="360" hidden="1">
       <c r="A103" s="13">
         <v>102</v>
       </c>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="O103" s="20"/>
     </row>
-    <row r="104" spans="1:15" ht="331.2" hidden="1">
+    <row r="104" spans="1:15" ht="360" hidden="1">
       <c r="A104" s="13">
         <v>103</v>
       </c>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="O104" s="20"/>
     </row>
-    <row r="105" spans="1:15" ht="302.39999999999998" hidden="1">
+    <row r="105" spans="1:15" ht="330" hidden="1">
       <c r="A105" s="13">
         <v>104</v>
       </c>
@@ -7207,7 +7207,7 @@
       </c>
       <c r="O105" s="20"/>
     </row>
-    <row r="106" spans="1:15" ht="331.2" hidden="1">
+    <row r="106" spans="1:15" ht="360" hidden="1">
       <c r="A106" s="13">
         <v>105</v>
       </c>
@@ -7236,7 +7236,7 @@
       </c>
       <c r="O106" s="20"/>
     </row>
-    <row r="107" spans="1:15" ht="331.2" hidden="1">
+    <row r="107" spans="1:15" ht="360" hidden="1">
       <c r="A107" s="13">
         <v>106</v>
       </c>
@@ -7265,7 +7265,7 @@
       </c>
       <c r="O107" s="20"/>
     </row>
-    <row r="108" spans="1:15" ht="316.8" hidden="1">
+    <row r="108" spans="1:15" ht="360" hidden="1">
       <c r="A108" s="13">
         <v>107</v>
       </c>
@@ -7294,7 +7294,7 @@
       </c>
       <c r="O108" s="20"/>
     </row>
-    <row r="109" spans="1:15" ht="316.8" hidden="1">
+    <row r="109" spans="1:15" ht="360" hidden="1">
       <c r="A109" s="13">
         <v>108</v>
       </c>
@@ -7323,7 +7323,7 @@
       </c>
       <c r="O109" s="20"/>
     </row>
-    <row r="110" spans="1:15" ht="316.8" hidden="1">
+    <row r="110" spans="1:15" ht="360" hidden="1">
       <c r="A110" s="13">
         <v>109</v>
       </c>
@@ -7352,7 +7352,7 @@
       </c>
       <c r="O110" s="20"/>
     </row>
-    <row r="111" spans="1:15" ht="302.39999999999998" hidden="1">
+    <row r="111" spans="1:15" ht="345" hidden="1">
       <c r="A111" s="13">
         <v>110</v>
       </c>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="O111" s="20"/>
     </row>
-    <row r="112" spans="1:15" ht="316.8" hidden="1">
+    <row r="112" spans="1:15" ht="360" hidden="1">
       <c r="A112" s="13">
         <v>111</v>
       </c>
@@ -7410,7 +7410,7 @@
       </c>
       <c r="O112" s="20"/>
     </row>
-    <row r="113" spans="1:15" ht="316.8" hidden="1">
+    <row r="113" spans="1:15" ht="360" hidden="1">
       <c r="A113" s="13">
         <v>112</v>
       </c>
@@ -7439,7 +7439,7 @@
       </c>
       <c r="O113" s="20"/>
     </row>
-    <row r="114" spans="1:15" ht="316.8" hidden="1">
+    <row r="114" spans="1:15" ht="360" hidden="1">
       <c r="A114" s="13">
         <v>113</v>
       </c>
@@ -7468,7 +7468,7 @@
       </c>
       <c r="O114" s="20"/>
     </row>
-    <row r="115" spans="1:15" ht="316.8" hidden="1">
+    <row r="115" spans="1:15" ht="360" hidden="1">
       <c r="A115" s="13">
         <v>114</v>
       </c>
@@ -7497,7 +7497,7 @@
       </c>
       <c r="O115" s="20"/>
     </row>
-    <row r="116" spans="1:15" ht="316.8" hidden="1">
+    <row r="116" spans="1:15" ht="360" hidden="1">
       <c r="A116" s="13">
         <v>115</v>
       </c>
@@ -7526,7 +7526,7 @@
       </c>
       <c r="O116" s="20"/>
     </row>
-    <row r="117" spans="1:15" ht="316.8" hidden="1">
+    <row r="117" spans="1:15" ht="360" hidden="1">
       <c r="A117" s="13">
         <v>116</v>
       </c>
@@ -7555,7 +7555,7 @@
       </c>
       <c r="O117" s="20"/>
     </row>
-    <row r="118" spans="1:15" ht="316.8" hidden="1">
+    <row r="118" spans="1:15" ht="360" hidden="1">
       <c r="A118" s="13">
         <v>117</v>
       </c>
@@ -7584,7 +7584,7 @@
       </c>
       <c r="O118" s="20"/>
     </row>
-    <row r="119" spans="1:15" ht="316.8" hidden="1">
+    <row r="119" spans="1:15" ht="360" hidden="1">
       <c r="A119" s="13">
         <v>118</v>
       </c>
@@ -7613,7 +7613,7 @@
       </c>
       <c r="O119" s="20"/>
     </row>
-    <row r="120" spans="1:15" ht="316.8" hidden="1">
+    <row r="120" spans="1:15" ht="360" hidden="1">
       <c r="A120" s="13">
         <v>119</v>
       </c>
@@ -7642,7 +7642,7 @@
       </c>
       <c r="O120" s="20"/>
     </row>
-    <row r="121" spans="1:15" ht="316.8" hidden="1">
+    <row r="121" spans="1:15" ht="360" hidden="1">
       <c r="A121" s="13">
         <v>120</v>
       </c>
@@ -7671,7 +7671,7 @@
       </c>
       <c r="O121" s="20"/>
     </row>
-    <row r="122" spans="1:15" ht="316.8" hidden="1">
+    <row r="122" spans="1:15" ht="360" hidden="1">
       <c r="A122" s="13">
         <v>121</v>
       </c>
@@ -7700,7 +7700,7 @@
       </c>
       <c r="O122" s="20"/>
     </row>
-    <row r="123" spans="1:15" ht="316.8" hidden="1">
+    <row r="123" spans="1:15" ht="330" hidden="1">
       <c r="A123" s="13">
         <v>122</v>
       </c>
@@ -7729,7 +7729,7 @@
       </c>
       <c r="O123" s="20"/>
     </row>
-    <row r="124" spans="1:15" ht="316.8" hidden="1">
+    <row r="124" spans="1:15" ht="330" hidden="1">
       <c r="A124" s="13">
         <v>123</v>
       </c>
@@ -7758,7 +7758,7 @@
       </c>
       <c r="O124" s="20"/>
     </row>
-    <row r="125" spans="1:15" ht="316.8" hidden="1">
+    <row r="125" spans="1:15" ht="330" hidden="1">
       <c r="A125" s="13">
         <v>124</v>
       </c>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="O125" s="20"/>
     </row>
-    <row r="126" spans="1:15" ht="331.2" hidden="1">
+    <row r="126" spans="1:15" ht="345" hidden="1">
       <c r="A126" s="13">
         <v>125</v>
       </c>
@@ -7816,7 +7816,7 @@
       </c>
       <c r="O126" s="20"/>
     </row>
-    <row r="127" spans="1:15" ht="316.8" hidden="1">
+    <row r="127" spans="1:15" ht="330" hidden="1">
       <c r="A127" s="13">
         <v>126</v>
       </c>
@@ -7845,7 +7845,7 @@
       </c>
       <c r="O127" s="20"/>
     </row>
-    <row r="128" spans="1:15" ht="316.8" hidden="1">
+    <row r="128" spans="1:15" ht="330" hidden="1">
       <c r="A128" s="13">
         <v>127</v>
       </c>
@@ -7874,7 +7874,7 @@
       </c>
       <c r="O128" s="20"/>
     </row>
-    <row r="129" spans="1:15" ht="316.8" hidden="1">
+    <row r="129" spans="1:15" ht="330" hidden="1">
       <c r="A129" s="13">
         <v>128</v>
       </c>
@@ -7903,7 +7903,7 @@
       </c>
       <c r="O129" s="20"/>
     </row>
-    <row r="130" spans="1:15" ht="331.2" hidden="1">
+    <row r="130" spans="1:15" ht="345" hidden="1">
       <c r="A130" s="13">
         <v>129</v>
       </c>
@@ -7932,7 +7932,7 @@
       </c>
       <c r="O130" s="20"/>
     </row>
-    <row r="131" spans="1:15" ht="316.8" hidden="1">
+    <row r="131" spans="1:15" ht="330" hidden="1">
       <c r="A131" s="13">
         <v>130</v>
       </c>
@@ -7961,7 +7961,7 @@
       </c>
       <c r="O131" s="20"/>
     </row>
-    <row r="132" spans="1:15" ht="316.8" hidden="1">
+    <row r="132" spans="1:15" ht="330" hidden="1">
       <c r="A132" s="13">
         <v>131</v>
       </c>
@@ -7990,7 +7990,7 @@
       </c>
       <c r="O132" s="20"/>
     </row>
-    <row r="133" spans="1:15" ht="316.8" hidden="1">
+    <row r="133" spans="1:15" ht="330" hidden="1">
       <c r="A133" s="13">
         <v>132</v>
       </c>
@@ -8019,7 +8019,7 @@
       </c>
       <c r="O133" s="20"/>
     </row>
-    <row r="134" spans="1:15" ht="331.2" hidden="1">
+    <row r="134" spans="1:15" ht="345" hidden="1">
       <c r="A134" s="13">
         <v>133</v>
       </c>
@@ -8048,7 +8048,7 @@
       </c>
       <c r="O134" s="20"/>
     </row>
-    <row r="135" spans="1:15" ht="316.8" hidden="1">
+    <row r="135" spans="1:15" ht="330" hidden="1">
       <c r="A135" s="13">
         <v>134</v>
       </c>
@@ -8077,7 +8077,7 @@
       </c>
       <c r="O135" s="20"/>
     </row>
-    <row r="136" spans="1:15" ht="316.8" hidden="1">
+    <row r="136" spans="1:15" ht="330" hidden="1">
       <c r="A136" s="13">
         <v>135</v>
       </c>
@@ -8106,7 +8106,7 @@
       </c>
       <c r="O136" s="20"/>
     </row>
-    <row r="137" spans="1:15" ht="316.8" hidden="1">
+    <row r="137" spans="1:15" ht="330" hidden="1">
       <c r="A137" s="13">
         <v>136</v>
       </c>
@@ -8135,7 +8135,7 @@
       </c>
       <c r="O137" s="20"/>
     </row>
-    <row r="138" spans="1:15" ht="331.2" hidden="1">
+    <row r="138" spans="1:15" ht="345" hidden="1">
       <c r="A138" s="13">
         <v>137</v>
       </c>
@@ -8164,7 +8164,7 @@
       </c>
       <c r="O138" s="20"/>
     </row>
-    <row r="139" spans="1:15" ht="316.8" hidden="1">
+    <row r="139" spans="1:15" ht="330" hidden="1">
       <c r="A139" s="13">
         <v>138</v>
       </c>
@@ -8193,7 +8193,7 @@
       </c>
       <c r="O139" s="20"/>
     </row>
-    <row r="140" spans="1:15" ht="316.8" hidden="1">
+    <row r="140" spans="1:15" ht="330" hidden="1">
       <c r="A140" s="13">
         <v>139</v>
       </c>
@@ -8222,7 +8222,7 @@
       </c>
       <c r="O140" s="20"/>
     </row>
-    <row r="141" spans="1:15" ht="316.8" hidden="1">
+    <row r="141" spans="1:15" ht="330" hidden="1">
       <c r="A141" s="13">
         <v>140</v>
       </c>
@@ -8251,7 +8251,7 @@
       </c>
       <c r="O141" s="20"/>
     </row>
-    <row r="142" spans="1:15" ht="331.2" hidden="1">
+    <row r="142" spans="1:15" ht="345" hidden="1">
       <c r="A142" s="13">
         <v>141</v>
       </c>
@@ -8280,7 +8280,7 @@
       </c>
       <c r="O142" s="20"/>
     </row>
-    <row r="143" spans="1:15" ht="316.8" hidden="1">
+    <row r="143" spans="1:15" ht="330" hidden="1">
       <c r="A143" s="13">
         <v>142</v>
       </c>
@@ -8309,7 +8309,7 @@
       </c>
       <c r="O143" s="20"/>
     </row>
-    <row r="144" spans="1:15" ht="316.8" hidden="1">
+    <row r="144" spans="1:15" ht="330" hidden="1">
       <c r="A144" s="13">
         <v>143</v>
       </c>
@@ -8338,7 +8338,7 @@
       </c>
       <c r="O144" s="20"/>
     </row>
-    <row r="145" spans="1:15" ht="316.8" hidden="1">
+    <row r="145" spans="1:15" ht="330" hidden="1">
       <c r="A145" s="13">
         <v>144</v>
       </c>
@@ -8367,7 +8367,7 @@
       </c>
       <c r="O145" s="20"/>
     </row>
-    <row r="146" spans="1:15" ht="331.2" hidden="1">
+    <row r="146" spans="1:15" ht="345" hidden="1">
       <c r="A146" s="13">
         <v>145</v>
       </c>
@@ -8396,7 +8396,7 @@
       </c>
       <c r="O146" s="20"/>
     </row>
-    <row r="147" spans="1:15" ht="331.2" hidden="1">
+    <row r="147" spans="1:15" ht="345" hidden="1">
       <c r="A147" s="13">
         <v>146</v>
       </c>
@@ -18615,13 +18615,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="58.44140625" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="58.42578125" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -19725,11 +19725,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>